<commit_message>
Fix send email to apptover
</commit_message>
<xml_diff>
--- a/BN/wwwroot/excel/Course_Assessment/Course_Assessment.xlsx
+++ b/BN/wwwroot/excel/Course_Assessment/Course_Assessment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10935" windowHeight="6765"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10935" windowHeight="6765" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ประเมินหลักสูตร" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
   <si>
     <t>แบบประเมินหลักสูตรการฝึกอบรม (Assessment Training Course)</t>
   </si>
@@ -446,6 +446,84 @@
   <si>
     <t>ผลรวม Total (คะแนนเต็ม 100 คะแนน)</t>
   </si>
+  <si>
+    <t>รหัสพนักงาน</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ตัวเลข 5  (ดีมาก </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Excellent)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ตัวเลข 2  (พอใช้ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fair) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ตัวเลข 4  (ดี </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good)     </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ตัวเลข 1  (ต้องปรับปรุง </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Need improvement) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ตัวเลข 3  (น่าพอใจ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Satisfactory)    </t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -454,7 +532,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +704,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Browallia New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -641,7 +733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1163,11 +1255,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1349,62 +1450,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1418,7 +1468,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1433,6 +1492,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1442,38 +1519,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,14 +1600,131 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1541,12 +1735,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1555,6 +1743,24 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1640,122 +1846,26 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1769,15 +1879,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2348,161 +2451,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="11262633" cy="582724"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="403225" y="3550104"/>
-          <a:ext cx="11262633" cy="582724"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>ตัวเลข 5  (ดีมาก </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Excellent)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>			ตัวเลข 4  (ดี </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Good)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>     </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>		    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>ตัวเลข 3  (น่าพอใจ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Satisfactory)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>	</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>ตัวเลข 2  (พอใช้ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Fair) 	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Browallia New" panose="020B0604020202020204" pitchFamily="34" charset="-34"/>
-            </a:rPr>
-            <a:t>		ตัวเลข 1  (ต้องปรับปรุง </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Need improvement) 	</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3116,7 +3064,7 @@
   </sheetPr>
   <dimension ref="B1:P999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
@@ -3139,21 +3087,21 @@
   <sheetData>
     <row r="1" spans="2:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
     </row>
     <row r="5" spans="2:14" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="39"/>
@@ -3171,23 +3119,23 @@
       <c r="N5" s="41"/>
     </row>
     <row r="6" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
       <c r="F6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="94"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="116"/>
+      <c r="M6" s="116"/>
+      <c r="N6" s="117"/>
     </row>
     <row r="7" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
@@ -3195,20 +3143,20 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="96"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="119"/>
     </row>
     <row r="8" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="120"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19" t="s">
@@ -3226,10 +3174,10 @@
       <c r="N8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="119" t="s">
+      <c r="B9" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="120"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -3275,89 +3223,89 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
     </row>
     <row r="13" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="97"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
     </row>
     <row r="14" spans="2:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110" t="s">
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="110" t="s">
+      <c r="H14" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="110" t="s">
+      <c r="I14" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="110" t="s">
+      <c r="J14" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="110" t="s">
+      <c r="K14" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="110" t="s">
+      <c r="L14" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="111"/>
-      <c r="N14" s="111"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
     </row>
     <row r="15" spans="2:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="110"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="111"/>
-      <c r="L15" s="111"/>
-      <c r="M15" s="111"/>
-      <c r="N15" s="111"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
     </row>
     <row r="16" spans="2:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="110"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="111"/>
       <c r="G16" s="31" t="s">
         <v>15</v>
       </c>
@@ -3373,9 +3321,9 @@
       <c r="K16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="121"/>
-      <c r="M16" s="121"/>
-      <c r="N16" s="121"/>
+      <c r="L16" s="113"/>
+      <c r="M16" s="113"/>
+      <c r="N16" s="113"/>
     </row>
     <row r="17" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="s">
@@ -3395,13 +3343,13 @@
       <c r="N17" s="17"/>
     </row>
     <row r="18" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="115"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -3412,13 +3360,13 @@
       <c r="N18" s="20"/>
     </row>
     <row r="19" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
@@ -3429,13 +3377,13 @@
       <c r="N19" s="20"/>
     </row>
     <row r="20" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -3446,11 +3394,11 @@
       <c r="N20" s="17"/>
     </row>
     <row r="21" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="106"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
@@ -3461,13 +3409,13 @@
       <c r="N21" s="20"/>
     </row>
     <row r="22" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="99"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -3478,11 +3426,11 @@
       <c r="N22" s="17"/>
     </row>
     <row r="23" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
@@ -3493,13 +3441,13 @@
       <c r="N23" s="20"/>
     </row>
     <row r="24" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -3510,11 +3458,11 @@
       <c r="N24" s="17"/>
     </row>
     <row r="25" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="100"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
@@ -3525,13 +3473,13 @@
       <c r="N25" s="20"/>
     </row>
     <row r="26" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
@@ -3542,13 +3490,13 @@
       <c r="N26" s="17"/>
     </row>
     <row r="27" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="114" t="s">
+      <c r="B27" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
@@ -3559,13 +3507,13 @@
       <c r="N27" s="20"/>
     </row>
     <row r="28" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -3576,13 +3524,13 @@
       <c r="N28" s="20"/>
     </row>
     <row r="29" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -3593,11 +3541,11 @@
       <c r="N29" s="17"/>
     </row>
     <row r="30" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="100"/>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
@@ -3608,13 +3556,13 @@
       <c r="N30" s="20"/>
     </row>
     <row r="31" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="102" t="s">
+      <c r="B31" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -3625,13 +3573,13 @@
       <c r="N31" s="17"/>
     </row>
     <row r="32" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="105"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
@@ -3642,13 +3590,13 @@
       <c r="N32" s="20"/>
     </row>
     <row r="33" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="110"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3894,72 +3842,72 @@
       <c r="N48" s="13"/>
     </row>
     <row r="49" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="97" t="s">
+      <c r="B49" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="97"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="97"/>
-      <c r="F49" s="97"/>
-      <c r="G49" s="97"/>
-      <c r="H49" s="97"/>
-      <c r="I49" s="97"/>
-      <c r="J49" s="97"/>
-      <c r="K49" s="97"/>
-      <c r="L49" s="97"/>
-      <c r="M49" s="97"/>
-      <c r="N49" s="97"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="102"/>
+      <c r="E49" s="102"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="102"/>
+      <c r="H49" s="102"/>
+      <c r="I49" s="102"/>
+      <c r="J49" s="102"/>
+      <c r="K49" s="102"/>
+      <c r="L49" s="102"/>
+      <c r="M49" s="102"/>
+      <c r="N49" s="102"/>
     </row>
     <row r="50" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="97" t="s">
+      <c r="B50" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="97"/>
-      <c r="D50" s="97"/>
-      <c r="E50" s="97"/>
-      <c r="F50" s="97"/>
-      <c r="G50" s="97"/>
-      <c r="H50" s="97"/>
-      <c r="I50" s="97"/>
-      <c r="J50" s="97"/>
-      <c r="K50" s="97"/>
-      <c r="L50" s="97"/>
-      <c r="M50" s="97"/>
-      <c r="N50" s="97"/>
+      <c r="C50" s="102"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="102"/>
+      <c r="F50" s="102"/>
+      <c r="G50" s="102"/>
+      <c r="H50" s="102"/>
+      <c r="I50" s="102"/>
+      <c r="J50" s="102"/>
+      <c r="K50" s="102"/>
+      <c r="L50" s="102"/>
+      <c r="M50" s="102"/>
+      <c r="N50" s="102"/>
     </row>
     <row r="51" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="97" t="s">
+      <c r="B51" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C51" s="97"/>
-      <c r="D51" s="97"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="97"/>
-      <c r="G51" s="97"/>
-      <c r="H51" s="97"/>
-      <c r="I51" s="97"/>
-      <c r="J51" s="97"/>
-      <c r="K51" s="97"/>
-      <c r="L51" s="97"/>
-      <c r="M51" s="97"/>
-      <c r="N51" s="97"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="102"/>
+      <c r="F51" s="102"/>
+      <c r="G51" s="102"/>
+      <c r="H51" s="102"/>
+      <c r="I51" s="102"/>
+      <c r="J51" s="102"/>
+      <c r="K51" s="102"/>
+      <c r="L51" s="102"/>
+      <c r="M51" s="102"/>
+      <c r="N51" s="102"/>
     </row>
     <row r="52" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="97" t="s">
+      <c r="B52" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="97"/>
-      <c r="D52" s="97"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="97"/>
-      <c r="G52" s="97"/>
-      <c r="H52" s="97"/>
-      <c r="I52" s="97"/>
-      <c r="J52" s="97"/>
-      <c r="K52" s="97"/>
-      <c r="L52" s="97"/>
-      <c r="M52" s="97"/>
-      <c r="N52" s="97"/>
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102"/>
+      <c r="F52" s="102"/>
+      <c r="G52" s="102"/>
+      <c r="H52" s="102"/>
+      <c r="I52" s="102"/>
+      <c r="J52" s="102"/>
+      <c r="K52" s="102"/>
+      <c r="L52" s="102"/>
+      <c r="M52" s="102"/>
+      <c r="N52" s="102"/>
     </row>
     <row r="53" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4910,6 +4858,22 @@
     <row r="999" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="G6:N6"/>
+    <mergeCell ref="G7:N7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B51:N51"/>
+    <mergeCell ref="B52:N52"/>
+    <mergeCell ref="B29:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B49:N49"/>
+    <mergeCell ref="B50:N50"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F21"/>
+    <mergeCell ref="B22:F23"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B28:F28"/>
@@ -4926,22 +4890,6 @@
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="L14:N16"/>
     <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G6:N6"/>
-    <mergeCell ref="G7:N7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B51:N51"/>
-    <mergeCell ref="B52:N52"/>
-    <mergeCell ref="B29:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B49:N49"/>
-    <mergeCell ref="B50:N50"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F21"/>
-    <mergeCell ref="B22:F23"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4957,7 +4905,7 @@
   <dimension ref="B4:X45"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection sqref="A1:X46"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4990,264 +4938,264 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:24" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="135"/>
-      <c r="Q4" s="135"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="135"/>
-      <c r="T4" s="135"/>
-      <c r="U4" s="135"/>
-      <c r="V4" s="135"/>
-      <c r="W4" s="135"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="127"/>
       <c r="X4" s="91"/>
     </row>
     <row r="5" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="125"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
-      <c r="Q5" s="125"/>
-      <c r="R5" s="125"/>
-      <c r="S5" s="125"/>
-      <c r="T5" s="125"/>
-      <c r="U5" s="125"/>
-      <c r="V5" s="125"/>
-      <c r="W5" s="125"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="126"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="126"/>
       <c r="X5" s="90"/>
     </row>
     <row r="6" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="125"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="125"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="125"/>
-      <c r="P6" s="125"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="125"/>
-      <c r="S6" s="125"/>
-      <c r="T6" s="125"/>
-      <c r="U6" s="125"/>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126"/>
+      <c r="R6" s="126"/>
+      <c r="S6" s="126"/>
+      <c r="T6" s="126"/>
+      <c r="U6" s="126"/>
+      <c r="V6" s="126"/>
+      <c r="W6" s="126"/>
       <c r="X6" s="90"/>
     </row>
     <row r="7" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="125"/>
-      <c r="T7" s="125"/>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="126"/>
+      <c r="T7" s="126"/>
+      <c r="U7" s="126"/>
+      <c r="V7" s="126"/>
+      <c r="W7" s="126"/>
       <c r="X7" s="90"/>
     </row>
     <row r="8" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="125"/>
-      <c r="N8" s="125"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="126"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="126"/>
+      <c r="T8" s="126"/>
+      <c r="U8" s="126"/>
+      <c r="V8" s="126"/>
+      <c r="W8" s="126"/>
       <c r="X8" s="90"/>
     </row>
     <row r="9" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="125"/>
-      <c r="J9" s="125"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="125"/>
-      <c r="M9" s="125"/>
-      <c r="N9" s="125"/>
-      <c r="O9" s="125"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="125"/>
-      <c r="R9" s="125"/>
-      <c r="S9" s="125"/>
-      <c r="T9" s="125"/>
-      <c r="U9" s="125"/>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="126"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="126"/>
+      <c r="Q9" s="126"/>
+      <c r="R9" s="126"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="126"/>
+      <c r="U9" s="126"/>
+      <c r="V9" s="126"/>
+      <c r="W9" s="126"/>
       <c r="X9" s="90"/>
     </row>
     <row r="10" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="125"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="125"/>
-      <c r="L10" s="125"/>
-      <c r="M10" s="125"/>
-      <c r="N10" s="125"/>
-      <c r="O10" s="125"/>
-      <c r="P10" s="125"/>
-      <c r="Q10" s="125"/>
-      <c r="R10" s="125"/>
-      <c r="S10" s="125"/>
-      <c r="T10" s="125"/>
-      <c r="U10" s="125"/>
-      <c r="V10" s="125"/>
-      <c r="W10" s="125"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
+      <c r="K10" s="126"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="126"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="126"/>
+      <c r="S10" s="126"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
+      <c r="V10" s="126"/>
+      <c r="W10" s="126"/>
       <c r="X10" s="90"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="125"/>
-      <c r="J11" s="125"/>
-      <c r="K11" s="125"/>
-      <c r="L11" s="125"/>
-      <c r="M11" s="125"/>
-      <c r="N11" s="125"/>
-      <c r="O11" s="125"/>
-      <c r="P11" s="125"/>
-      <c r="Q11" s="125"/>
-      <c r="R11" s="125"/>
-      <c r="S11" s="125"/>
-      <c r="T11" s="125"/>
-      <c r="U11" s="125"/>
-      <c r="V11" s="125"/>
-      <c r="W11" s="125"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="126"/>
+      <c r="O11" s="126"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="126"/>
+      <c r="R11" s="126"/>
+      <c r="S11" s="126"/>
+      <c r="T11" s="126"/>
+      <c r="U11" s="126"/>
+      <c r="V11" s="126"/>
+      <c r="W11" s="126"/>
       <c r="X11" s="90"/>
     </row>
     <row r="12" spans="2:24" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="126"/>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="126"/>
-      <c r="N12" s="126"/>
-      <c r="O12" s="126"/>
-      <c r="P12" s="126"/>
-      <c r="Q12" s="126"/>
-      <c r="R12" s="126"/>
-      <c r="S12" s="126"/>
-      <c r="T12" s="126"/>
-      <c r="U12" s="126"/>
-      <c r="V12" s="126"/>
-      <c r="W12" s="126"/>
-      <c r="X12" s="234"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="150"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="150"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="150"/>
+      <c r="L12" s="150"/>
+      <c r="M12" s="150"/>
+      <c r="N12" s="150"/>
+      <c r="O12" s="150"/>
+      <c r="P12" s="150"/>
+      <c r="Q12" s="150"/>
+      <c r="R12" s="150"/>
+      <c r="S12" s="150"/>
+      <c r="T12" s="150"/>
+      <c r="U12" s="150"/>
+      <c r="V12" s="150"/>
+      <c r="W12" s="150"/>
+      <c r="X12" s="93"/>
     </row>
     <row r="13" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="137"/>
-      <c r="D13" s="142" t="s">
+      <c r="C13" s="129"/>
+      <c r="D13" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="143"/>
-      <c r="M13" s="143"/>
-      <c r="N13" s="143"/>
-      <c r="O13" s="143"/>
-      <c r="P13" s="143"/>
-      <c r="Q13" s="143"/>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
-      <c r="T13" s="143"/>
-      <c r="U13" s="143"/>
-      <c r="V13" s="143"/>
-      <c r="W13" s="144"/>
-      <c r="X13" s="235"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="135"/>
+      <c r="J13" s="135"/>
+      <c r="K13" s="135"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="135"/>
+      <c r="O13" s="135"/>
+      <c r="P13" s="135"/>
+      <c r="Q13" s="135"/>
+      <c r="R13" s="135"/>
+      <c r="S13" s="135"/>
+      <c r="T13" s="135"/>
+      <c r="U13" s="135"/>
+      <c r="V13" s="135"/>
+      <c r="W13" s="136"/>
+      <c r="X13" s="94"/>
     </row>
     <row r="14" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="138"/>
-      <c r="C14" s="139"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="131"/>
       <c r="D14" s="87" t="s">
         <v>108</v>
       </c>
@@ -5291,8 +5239,8 @@
       <c r="X14" s="89"/>
     </row>
     <row r="15" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="138"/>
-      <c r="C15" s="139"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="131"/>
       <c r="D15" s="21" t="s">
         <v>41</v>
       </c>
@@ -5336,8 +5284,8 @@
       <c r="X15" s="14"/>
     </row>
     <row r="16" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="140"/>
-      <c r="C16" s="141"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="133"/>
       <c r="D16" s="26" t="s">
         <v>42</v>
       </c>
@@ -5381,10 +5329,10 @@
       <c r="X16" s="14"/>
     </row>
     <row r="17" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="145" t="s">
+      <c r="B17" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="146"/>
+      <c r="C17" s="138"/>
       <c r="D17" s="7"/>
       <c r="E17" s="1"/>
       <c r="F17" s="7"/>
@@ -5408,8 +5356,8 @@
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="147"/>
-      <c r="C18" s="148"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="140"/>
       <c r="D18" s="10"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
@@ -5433,8 +5381,8 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="149"/>
-      <c r="C19" s="150"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="142"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
@@ -5458,10 +5406,10 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="127" t="s">
+      <c r="B20" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="128"/>
+      <c r="C20" s="144"/>
       <c r="D20" s="7"/>
       <c r="E20" s="1"/>
       <c r="F20" s="7"/>
@@ -5485,8 +5433,8 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="129"/>
-      <c r="C21" s="130"/>
+      <c r="B21" s="145"/>
+      <c r="C21" s="146"/>
       <c r="D21" s="10"/>
       <c r="E21" s="3"/>
       <c r="F21" s="10"/>
@@ -5510,8 +5458,8 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="131"/>
-      <c r="C22" s="132"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="148"/>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
@@ -5535,10 +5483,10 @@
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="127" t="s">
+      <c r="B23" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="128"/>
+      <c r="C23" s="144"/>
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
       <c r="F23" s="7"/>
@@ -5562,8 +5510,8 @@
       <c r="X23" s="2"/>
     </row>
     <row r="24" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="129"/>
-      <c r="C24" s="130"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="146"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3"/>
       <c r="F24" s="10"/>
@@ -5587,8 +5535,8 @@
       <c r="X24" s="2"/>
     </row>
     <row r="25" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="131"/>
-      <c r="C25" s="132"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="148"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="4"/>
@@ -5612,10 +5560,10 @@
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="127" t="s">
+      <c r="B26" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="128"/>
+      <c r="C26" s="144"/>
       <c r="D26" s="7"/>
       <c r="E26" s="1"/>
       <c r="F26" s="7"/>
@@ -5639,8 +5587,8 @@
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="129"/>
-      <c r="C27" s="130"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="146"/>
       <c r="D27" s="10"/>
       <c r="E27" s="3"/>
       <c r="F27" s="10"/>
@@ -5664,8 +5612,8 @@
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="131"/>
-      <c r="C28" s="132"/>
+      <c r="B28" s="147"/>
+      <c r="C28" s="148"/>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
@@ -5689,10 +5637,10 @@
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="127" t="s">
+      <c r="B29" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="128"/>
+      <c r="C29" s="144"/>
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
       <c r="F29" s="7"/>
@@ -5716,8 +5664,8 @@
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="129"/>
-      <c r="C30" s="130"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
       <c r="D30" s="10"/>
       <c r="E30" s="3"/>
       <c r="F30" s="10"/>
@@ -5741,8 +5689,8 @@
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="131"/>
-      <c r="C31" s="132"/>
+      <c r="B31" s="147"/>
+      <c r="C31" s="148"/>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
@@ -5766,10 +5714,10 @@
       <c r="X31" s="2"/>
     </row>
     <row r="32" spans="2:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="133" t="s">
+      <c r="B32" s="151" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="134"/>
+      <c r="C32" s="152"/>
       <c r="D32" s="11"/>
       <c r="E32" s="8"/>
       <c r="F32" s="12"/>
@@ -5948,120 +5896,115 @@
       <c r="X40" s="84"/>
     </row>
     <row r="42" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="124"/>
-      <c r="D42" s="124"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="124"/>
-      <c r="G42" s="124"/>
-      <c r="H42" s="124"/>
-      <c r="I42" s="124"/>
-      <c r="J42" s="124"/>
-      <c r="K42" s="124"/>
-      <c r="L42" s="124"/>
-      <c r="M42" s="124"/>
-      <c r="N42" s="124"/>
-      <c r="O42" s="124"/>
-      <c r="P42" s="124"/>
-      <c r="Q42" s="124"/>
-      <c r="R42" s="124"/>
-      <c r="S42" s="124"/>
-      <c r="T42" s="124"/>
-      <c r="U42" s="124"/>
-      <c r="V42" s="124"/>
-      <c r="W42" s="124"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="149"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="149"/>
+      <c r="G42" s="149"/>
+      <c r="H42" s="149"/>
+      <c r="I42" s="149"/>
+      <c r="J42" s="149"/>
+      <c r="K42" s="149"/>
+      <c r="L42" s="149"/>
+      <c r="M42" s="149"/>
+      <c r="N42" s="149"/>
+      <c r="O42" s="149"/>
+      <c r="P42" s="149"/>
+      <c r="Q42" s="149"/>
+      <c r="R42" s="149"/>
+      <c r="S42" s="149"/>
+      <c r="T42" s="149"/>
+      <c r="U42" s="149"/>
+      <c r="V42" s="149"/>
+      <c r="W42" s="149"/>
       <c r="X42" s="92"/>
     </row>
     <row r="43" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="124" t="s">
+      <c r="B43" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="124"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="124"/>
-      <c r="H43" s="124"/>
-      <c r="I43" s="124"/>
-      <c r="J43" s="124"/>
-      <c r="K43" s="124"/>
-      <c r="L43" s="124"/>
-      <c r="M43" s="124"/>
-      <c r="N43" s="124"/>
-      <c r="O43" s="124"/>
-      <c r="P43" s="124"/>
-      <c r="Q43" s="124"/>
-      <c r="R43" s="124"/>
-      <c r="S43" s="124"/>
-      <c r="T43" s="124"/>
-      <c r="U43" s="124"/>
-      <c r="V43" s="124"/>
-      <c r="W43" s="124"/>
+      <c r="C43" s="149"/>
+      <c r="D43" s="149"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="149"/>
+      <c r="G43" s="149"/>
+      <c r="H43" s="149"/>
+      <c r="I43" s="149"/>
+      <c r="J43" s="149"/>
+      <c r="K43" s="149"/>
+      <c r="L43" s="149"/>
+      <c r="M43" s="149"/>
+      <c r="N43" s="149"/>
+      <c r="O43" s="149"/>
+      <c r="P43" s="149"/>
+      <c r="Q43" s="149"/>
+      <c r="R43" s="149"/>
+      <c r="S43" s="149"/>
+      <c r="T43" s="149"/>
+      <c r="U43" s="149"/>
+      <c r="V43" s="149"/>
+      <c r="W43" s="149"/>
       <c r="X43" s="92"/>
     </row>
     <row r="44" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="124" t="s">
+      <c r="B44" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="124"/>
-      <c r="D44" s="124"/>
-      <c r="E44" s="124"/>
-      <c r="F44" s="124"/>
-      <c r="G44" s="124"/>
-      <c r="H44" s="124"/>
-      <c r="I44" s="124"/>
-      <c r="J44" s="124"/>
-      <c r="K44" s="124"/>
-      <c r="L44" s="124"/>
-      <c r="M44" s="124"/>
-      <c r="N44" s="124"/>
-      <c r="O44" s="124"/>
-      <c r="P44" s="124"/>
-      <c r="Q44" s="124"/>
-      <c r="R44" s="124"/>
-      <c r="S44" s="124"/>
-      <c r="T44" s="124"/>
-      <c r="U44" s="124"/>
-      <c r="V44" s="124"/>
-      <c r="W44" s="124"/>
+      <c r="C44" s="149"/>
+      <c r="D44" s="149"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="149"/>
+      <c r="G44" s="149"/>
+      <c r="H44" s="149"/>
+      <c r="I44" s="149"/>
+      <c r="J44" s="149"/>
+      <c r="K44" s="149"/>
+      <c r="L44" s="149"/>
+      <c r="M44" s="149"/>
+      <c r="N44" s="149"/>
+      <c r="O44" s="149"/>
+      <c r="P44" s="149"/>
+      <c r="Q44" s="149"/>
+      <c r="R44" s="149"/>
+      <c r="S44" s="149"/>
+      <c r="T44" s="149"/>
+      <c r="U44" s="149"/>
+      <c r="V44" s="149"/>
+      <c r="W44" s="149"/>
       <c r="X44" s="92"/>
     </row>
     <row r="45" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="124" t="s">
+      <c r="B45" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="124"/>
-      <c r="D45" s="124"/>
-      <c r="E45" s="124"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="124"/>
-      <c r="I45" s="124"/>
-      <c r="J45" s="124"/>
-      <c r="K45" s="124"/>
-      <c r="L45" s="124"/>
-      <c r="M45" s="124"/>
-      <c r="N45" s="124"/>
-      <c r="O45" s="124"/>
-      <c r="P45" s="124"/>
-      <c r="Q45" s="124"/>
-      <c r="R45" s="124"/>
-      <c r="S45" s="124"/>
-      <c r="T45" s="124"/>
-      <c r="U45" s="124"/>
-      <c r="V45" s="124"/>
-      <c r="W45" s="124"/>
+      <c r="C45" s="149"/>
+      <c r="D45" s="149"/>
+      <c r="E45" s="149"/>
+      <c r="F45" s="149"/>
+      <c r="G45" s="149"/>
+      <c r="H45" s="149"/>
+      <c r="I45" s="149"/>
+      <c r="J45" s="149"/>
+      <c r="K45" s="149"/>
+      <c r="L45" s="149"/>
+      <c r="M45" s="149"/>
+      <c r="N45" s="149"/>
+      <c r="O45" s="149"/>
+      <c r="P45" s="149"/>
+      <c r="Q45" s="149"/>
+      <c r="R45" s="149"/>
+      <c r="S45" s="149"/>
+      <c r="T45" s="149"/>
+      <c r="U45" s="149"/>
+      <c r="V45" s="149"/>
+      <c r="W45" s="149"/>
       <c r="X45" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B4:W4"/>
-    <mergeCell ref="B13:C16"/>
-    <mergeCell ref="D13:W13"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="B20:C22"/>
     <mergeCell ref="B44:W44"/>
     <mergeCell ref="B45:W45"/>
     <mergeCell ref="B5:W12"/>
@@ -6071,6 +6014,11 @@
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B42:W42"/>
     <mergeCell ref="B43:W43"/>
+    <mergeCell ref="B4:W4"/>
+    <mergeCell ref="B13:C16"/>
+    <mergeCell ref="D13:W13"/>
+    <mergeCell ref="B17:C19"/>
+    <mergeCell ref="B20:C22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -6085,8 +6033,8 @@
   </sheetPr>
   <dimension ref="B1:M999"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:H31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6106,23 +6054,30 @@
     <col min="14" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="236"/>
+    </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="197" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
     </row>
     <row r="5" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
@@ -6138,21 +6093,21 @@
       <c r="L5" s="17"/>
     </row>
     <row r="6" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="164" t="s">
+      <c r="B6" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="165"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="153"/>
+      <c r="C6" s="200"/>
+      <c r="D6" s="227"/>
+      <c r="E6" s="227"/>
       <c r="F6" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="196"/>
+      <c r="G6" s="227"/>
+      <c r="H6" s="227"/>
+      <c r="I6" s="227"/>
+      <c r="J6" s="227"/>
+      <c r="K6" s="227"/>
+      <c r="L6" s="228"/>
     </row>
     <row r="7" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="77"/>
@@ -6160,48 +6115,48 @@
       <c r="D7" s="76"/>
       <c r="E7" s="76"/>
       <c r="F7" s="76"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="151"/>
-      <c r="I7" s="151"/>
-      <c r="J7" s="151"/>
-      <c r="K7" s="151"/>
-      <c r="L7" s="152"/>
+      <c r="G7" s="229"/>
+      <c r="H7" s="229"/>
+      <c r="I7" s="229"/>
+      <c r="J7" s="229"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="230"/>
     </row>
     <row r="8" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="78" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="76"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="153"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
       <c r="F8" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
+      <c r="G8" s="229"/>
+      <c r="H8" s="229"/>
       <c r="I8" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="151"/>
-      <c r="K8" s="151"/>
-      <c r="L8" s="152"/>
+      <c r="J8" s="229"/>
+      <c r="K8" s="229"/>
+      <c r="L8" s="230"/>
     </row>
     <row r="9" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="76"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
+      <c r="D9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="227"/>
+      <c r="H9" s="227"/>
       <c r="I9" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="151"/>
-      <c r="K9" s="151"/>
-      <c r="L9" s="152"/>
+      <c r="J9" s="229"/>
+      <c r="K9" s="229"/>
+      <c r="L9" s="230"/>
     </row>
     <row r="10" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="26"/>
@@ -6218,186 +6173,202 @@
     </row>
     <row r="11" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="166" t="s">
+      <c r="B12" s="201" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="166"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="166"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="166"/>
-      <c r="K12" s="166"/>
-      <c r="L12" s="166"/>
-      <c r="M12" s="166"/>
+      <c r="C12" s="201"/>
+      <c r="D12" s="201"/>
+      <c r="E12" s="201"/>
+      <c r="F12" s="201"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="201"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="201"/>
+      <c r="K12" s="201"/>
+      <c r="L12" s="201"/>
+      <c r="M12" s="201"/>
     </row>
-    <row r="13" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="237" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="237" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="237" t="s">
+        <v>115</v>
+      </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="237" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="237" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="15" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="167" t="s">
+      <c r="B16" s="202" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="168"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="168"/>
-      <c r="F16" s="168"/>
-      <c r="G16" s="169"/>
-      <c r="H16" s="176" t="s">
+      <c r="C16" s="203"/>
+      <c r="D16" s="203"/>
+      <c r="E16" s="203"/>
+      <c r="F16" s="203"/>
+      <c r="G16" s="204"/>
+      <c r="H16" s="211" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="179" t="s">
+      <c r="I16" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="180"/>
-      <c r="K16" s="180"/>
-      <c r="L16" s="181"/>
+      <c r="J16" s="215"/>
+      <c r="K16" s="215"/>
+      <c r="L16" s="216"/>
     </row>
     <row r="17" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="170"/>
-      <c r="C17" s="171"/>
-      <c r="D17" s="171"/>
-      <c r="E17" s="171"/>
-      <c r="F17" s="171"/>
-      <c r="G17" s="172"/>
-      <c r="H17" s="177"/>
-      <c r="I17" s="138"/>
-      <c r="J17" s="182"/>
-      <c r="K17" s="182"/>
-      <c r="L17" s="183"/>
+      <c r="B17" s="205"/>
+      <c r="C17" s="206"/>
+      <c r="D17" s="206"/>
+      <c r="E17" s="206"/>
+      <c r="F17" s="206"/>
+      <c r="G17" s="207"/>
+      <c r="H17" s="212"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="217"/>
+      <c r="K17" s="217"/>
+      <c r="L17" s="218"/>
     </row>
     <row r="18" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="173"/>
-      <c r="C18" s="174"/>
-      <c r="D18" s="174"/>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="175"/>
-      <c r="H18" s="178"/>
-      <c r="I18" s="184"/>
-      <c r="J18" s="185"/>
-      <c r="K18" s="185"/>
-      <c r="L18" s="186"/>
+      <c r="B18" s="208"/>
+      <c r="C18" s="209"/>
+      <c r="D18" s="209"/>
+      <c r="E18" s="209"/>
+      <c r="F18" s="209"/>
+      <c r="G18" s="210"/>
+      <c r="H18" s="213"/>
+      <c r="I18" s="219"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="220"/>
+      <c r="L18" s="221"/>
     </row>
     <row r="19" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="187" t="s">
+      <c r="B19" s="222" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="188"/>
-      <c r="D19" s="188"/>
-      <c r="E19" s="188"/>
-      <c r="F19" s="188"/>
-      <c r="G19" s="189"/>
-      <c r="H19" s="190"/>
+      <c r="C19" s="223"/>
+      <c r="D19" s="223"/>
+      <c r="E19" s="223"/>
+      <c r="F19" s="223"/>
+      <c r="G19" s="224"/>
+      <c r="H19" s="161"/>
       <c r="I19" s="42"/>
       <c r="J19" s="43"/>
       <c r="K19" s="43"/>
       <c r="L19" s="44"/>
     </row>
     <row r="20" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="192" t="s">
+      <c r="B20" s="225" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="193"/>
-      <c r="D20" s="193"/>
-      <c r="E20" s="193"/>
-      <c r="F20" s="193"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="191"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
+      <c r="E20" s="226"/>
+      <c r="F20" s="226"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="162"/>
       <c r="I20" s="45"/>
       <c r="J20" s="46"/>
       <c r="K20" s="46"/>
       <c r="L20" s="47"/>
     </row>
     <row r="21" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="195"/>
-      <c r="D21" s="195"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="132"/>
-      <c r="H21" s="158"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="168"/>
+      <c r="F21" s="168"/>
+      <c r="G21" s="148"/>
+      <c r="H21" s="163"/>
       <c r="I21" s="45"/>
       <c r="J21" s="46"/>
       <c r="K21" s="46"/>
       <c r="L21" s="47"/>
     </row>
     <row r="22" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="157"/>
+      <c r="C22" s="186"/>
+      <c r="D22" s="186"/>
+      <c r="E22" s="186"/>
+      <c r="F22" s="186"/>
+      <c r="G22" s="187"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="48"/>
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
       <c r="L22" s="50"/>
     </row>
     <row r="23" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="159" t="s">
+      <c r="B23" s="188" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="160"/>
-      <c r="D23" s="160"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="158"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="189"/>
+      <c r="F23" s="189"/>
+      <c r="G23" s="190"/>
+      <c r="H23" s="163"/>
       <c r="I23" s="51"/>
       <c r="J23" s="52"/>
       <c r="K23" s="52"/>
       <c r="L23" s="53"/>
     </row>
     <row r="24" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="157"/>
+      <c r="C24" s="186"/>
+      <c r="D24" s="186"/>
+      <c r="E24" s="186"/>
+      <c r="F24" s="186"/>
+      <c r="G24" s="187"/>
+      <c r="H24" s="169"/>
       <c r="I24" s="48"/>
       <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="L24" s="50"/>
     </row>
     <row r="25" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="159" t="s">
+      <c r="B25" s="188" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="160"/>
-      <c r="D25" s="160"/>
-      <c r="E25" s="160"/>
-      <c r="F25" s="160"/>
-      <c r="G25" s="161"/>
-      <c r="H25" s="158"/>
+      <c r="C25" s="189"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="189"/>
+      <c r="F25" s="189"/>
+      <c r="G25" s="190"/>
+      <c r="H25" s="163"/>
       <c r="I25" s="51"/>
       <c r="J25" s="52"/>
       <c r="K25" s="52"/>
       <c r="L25" s="53"/>
     </row>
     <row r="26" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="197" t="s">
+      <c r="B26" s="191" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="198"/>
-      <c r="D26" s="198"/>
-      <c r="E26" s="198"/>
-      <c r="F26" s="198"/>
-      <c r="G26" s="199"/>
-      <c r="H26" s="157"/>
+      <c r="C26" s="192"/>
+      <c r="D26" s="192"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="169"/>
       <c r="I26" s="48" t="s">
         <v>59</v>
       </c>
@@ -6406,224 +6377,224 @@
       <c r="L26" s="50"/>
     </row>
     <row r="27" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="200" t="s">
+      <c r="B27" s="182" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="201"/>
-      <c r="D27" s="201"/>
-      <c r="E27" s="201"/>
-      <c r="F27" s="201"/>
-      <c r="G27" s="202"/>
-      <c r="H27" s="158"/>
+      <c r="C27" s="183"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="183"/>
+      <c r="F27" s="183"/>
+      <c r="G27" s="184"/>
+      <c r="H27" s="163"/>
       <c r="I27" s="51"/>
       <c r="J27" s="52"/>
       <c r="K27" s="52"/>
       <c r="L27" s="53"/>
     </row>
     <row r="28" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="208"/>
-      <c r="D28" s="208"/>
-      <c r="E28" s="208"/>
-      <c r="F28" s="208"/>
-      <c r="G28" s="128"/>
-      <c r="H28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="169"/>
       <c r="I28" s="48"/>
       <c r="J28" s="49"/>
       <c r="K28" s="49"/>
       <c r="L28" s="50"/>
     </row>
     <row r="29" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="200" t="s">
+      <c r="B29" s="182" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="201"/>
-      <c r="D29" s="201"/>
-      <c r="E29" s="201"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="202"/>
-      <c r="H29" s="158"/>
+      <c r="C29" s="183"/>
+      <c r="D29" s="183"/>
+      <c r="E29" s="183"/>
+      <c r="F29" s="183"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="163"/>
       <c r="I29" s="51"/>
       <c r="J29" s="52"/>
       <c r="K29" s="52"/>
       <c r="L29" s="53"/>
     </row>
     <row r="30" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="154" t="s">
+      <c r="B30" s="185" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="156"/>
-      <c r="H30" s="157"/>
+      <c r="C30" s="186"/>
+      <c r="D30" s="186"/>
+      <c r="E30" s="186"/>
+      <c r="F30" s="186"/>
+      <c r="G30" s="187"/>
+      <c r="H30" s="169"/>
       <c r="I30" s="54"/>
       <c r="J30" s="55"/>
       <c r="K30" s="55"/>
       <c r="L30" s="56"/>
     </row>
     <row r="31" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="159" t="s">
+      <c r="B31" s="188" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="160"/>
-      <c r="D31" s="160"/>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
-      <c r="G31" s="161"/>
-      <c r="H31" s="158"/>
+      <c r="C31" s="189"/>
+      <c r="D31" s="189"/>
+      <c r="E31" s="189"/>
+      <c r="F31" s="189"/>
+      <c r="G31" s="190"/>
+      <c r="H31" s="163"/>
       <c r="I31" s="54"/>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
       <c r="L31" s="56"/>
     </row>
     <row r="32" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="197" t="s">
+      <c r="B32" s="191" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="198"/>
-      <c r="D32" s="198"/>
-      <c r="E32" s="198"/>
-      <c r="F32" s="198"/>
-      <c r="G32" s="199"/>
-      <c r="H32" s="157"/>
+      <c r="C32" s="192"/>
+      <c r="D32" s="192"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="169"/>
       <c r="I32" s="48"/>
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
       <c r="L32" s="50"/>
     </row>
     <row r="33" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="200" t="s">
+      <c r="B33" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="201"/>
-      <c r="D33" s="201"/>
-      <c r="E33" s="201"/>
-      <c r="F33" s="201"/>
-      <c r="G33" s="202"/>
-      <c r="H33" s="191"/>
+      <c r="C33" s="183"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="183"/>
+      <c r="F33" s="183"/>
+      <c r="G33" s="184"/>
+      <c r="H33" s="162"/>
       <c r="I33" s="45"/>
       <c r="J33" s="46"/>
       <c r="K33" s="46"/>
       <c r="L33" s="47"/>
     </row>
     <row r="34" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="197" t="s">
+      <c r="B34" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="198"/>
-      <c r="D34" s="198"/>
-      <c r="E34" s="198"/>
-      <c r="F34" s="198"/>
-      <c r="G34" s="199"/>
-      <c r="H34" s="157"/>
+      <c r="C34" s="192"/>
+      <c r="D34" s="192"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="169"/>
       <c r="I34" s="48"/>
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
       <c r="L34" s="50"/>
     </row>
     <row r="35" spans="2:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="204" t="s">
+      <c r="B35" s="194" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="205"/>
-      <c r="D35" s="205"/>
-      <c r="E35" s="205"/>
-      <c r="F35" s="205"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="203"/>
+      <c r="C35" s="195"/>
+      <c r="D35" s="195"/>
+      <c r="E35" s="195"/>
+      <c r="F35" s="195"/>
+      <c r="G35" s="196"/>
+      <c r="H35" s="170"/>
       <c r="I35" s="57"/>
       <c r="J35" s="58"/>
       <c r="K35" s="58"/>
       <c r="L35" s="59"/>
     </row>
     <row r="36" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="212" t="s">
+      <c r="B36" s="158" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="213"/>
-      <c r="D36" s="213"/>
-      <c r="E36" s="213"/>
-      <c r="F36" s="213"/>
-      <c r="G36" s="214"/>
-      <c r="H36" s="190"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="160"/>
+      <c r="H36" s="161"/>
       <c r="I36" s="42"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
       <c r="L36" s="44"/>
     </row>
     <row r="37" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="215" t="s">
+      <c r="B37" s="164" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="216"/>
-      <c r="D37" s="216"/>
-      <c r="E37" s="216"/>
-      <c r="F37" s="216"/>
-      <c r="G37" s="217"/>
-      <c r="H37" s="191"/>
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="165"/>
+      <c r="F37" s="165"/>
+      <c r="G37" s="166"/>
+      <c r="H37" s="162"/>
       <c r="I37" s="45"/>
       <c r="J37" s="46"/>
       <c r="K37" s="46"/>
       <c r="L37" s="47"/>
     </row>
     <row r="38" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="194" t="s">
+      <c r="B38" s="167" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="195"/>
-      <c r="D38" s="195"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="132"/>
-      <c r="H38" s="158"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="168"/>
+      <c r="E38" s="168"/>
+      <c r="F38" s="168"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="163"/>
       <c r="I38" s="51"/>
       <c r="J38" s="52"/>
       <c r="K38" s="52"/>
       <c r="L38" s="53"/>
     </row>
     <row r="39" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="207" t="s">
+      <c r="B39" s="156" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="208"/>
-      <c r="D39" s="208"/>
-      <c r="E39" s="208"/>
-      <c r="F39" s="208"/>
-      <c r="G39" s="128"/>
-      <c r="H39" s="157"/>
+      <c r="C39" s="157"/>
+      <c r="D39" s="157"/>
+      <c r="E39" s="157"/>
+      <c r="F39" s="157"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="169"/>
       <c r="I39" s="48"/>
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
       <c r="L39" s="50"/>
     </row>
     <row r="40" spans="2:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="218" t="s">
+      <c r="B40" s="171" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="219"/>
-      <c r="D40" s="219"/>
-      <c r="E40" s="219"/>
-      <c r="F40" s="219"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="203"/>
+      <c r="C40" s="172"/>
+      <c r="D40" s="172"/>
+      <c r="E40" s="172"/>
+      <c r="F40" s="172"/>
+      <c r="G40" s="173"/>
+      <c r="H40" s="170"/>
       <c r="I40" s="57"/>
       <c r="J40" s="58"/>
       <c r="K40" s="58"/>
       <c r="L40" s="59"/>
     </row>
     <row r="41" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="221" t="s">
+      <c r="B41" s="174" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="222"/>
-      <c r="D41" s="222"/>
-      <c r="E41" s="222"/>
-      <c r="F41" s="222"/>
-      <c r="G41" s="223"/>
+      <c r="C41" s="175"/>
+      <c r="D41" s="175"/>
+      <c r="E41" s="175"/>
+      <c r="F41" s="175"/>
+      <c r="G41" s="176"/>
       <c r="H41" s="60"/>
       <c r="I41" s="61"/>
       <c r="J41" s="62"/>
@@ -6653,14 +6624,14 @@
       <c r="L43" s="14"/>
     </row>
     <row r="44" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="224" t="s">
+      <c r="B44" s="177" t="s">
         <v>74</v>
       </c>
-      <c r="C44" s="225"/>
-      <c r="D44" s="225"/>
-      <c r="E44" s="225"/>
-      <c r="F44" s="225"/>
-      <c r="G44" s="226"/>
+      <c r="C44" s="178"/>
+      <c r="D44" s="178"/>
+      <c r="E44" s="178"/>
+      <c r="F44" s="178"/>
+      <c r="G44" s="179"/>
       <c r="H44" s="72"/>
       <c r="I44" s="42"/>
       <c r="J44" s="43"/>
@@ -6668,14 +6639,14 @@
       <c r="L44" s="44"/>
     </row>
     <row r="45" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="227" t="s">
+      <c r="B45" s="180" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="228"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="181"/>
       <c r="H45" s="73"/>
       <c r="I45" s="45"/>
       <c r="J45" s="46"/>
@@ -6683,14 +6654,14 @@
       <c r="L45" s="47"/>
     </row>
     <row r="46" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="209" t="s">
+      <c r="B46" s="153" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="210"/>
-      <c r="D46" s="210"/>
-      <c r="E46" s="210"/>
-      <c r="F46" s="210"/>
-      <c r="G46" s="211"/>
+      <c r="C46" s="154"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="154"/>
+      <c r="G46" s="155"/>
       <c r="H46" s="74"/>
       <c r="I46" s="57"/>
       <c r="J46" s="58"/>
@@ -7704,35 +7675,11 @@
     <row r="999" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="J9:L9"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="B23:G23"/>
@@ -7749,11 +7696,35 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7786,21 +7757,21 @@
   <sheetData>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="230" t="s">
+      <c r="B4" s="233" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="230"/>
-      <c r="D4" s="230"/>
-      <c r="E4" s="230"/>
-      <c r="F4" s="230"/>
-      <c r="G4" s="230"/>
-      <c r="H4" s="230"/>
-      <c r="I4" s="230"/>
-      <c r="J4" s="230"/>
-      <c r="K4" s="230"/>
-      <c r="L4" s="230"/>
-      <c r="M4" s="230"/>
-      <c r="N4" s="230"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
+      <c r="F4" s="233"/>
+      <c r="G4" s="233"/>
+      <c r="H4" s="233"/>
+      <c r="I4" s="233"/>
+      <c r="J4" s="233"/>
+      <c r="K4" s="233"/>
+      <c r="L4" s="233"/>
+      <c r="M4" s="233"/>
+      <c r="N4" s="233"/>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7826,59 +7797,59 @@
         <v>1</v>
       </c>
       <c r="C8" s="76"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="153"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
       <c r="F8" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="196"/>
+      <c r="G8" s="227"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="227"/>
+      <c r="K8" s="227"/>
+      <c r="L8" s="227"/>
+      <c r="M8" s="227"/>
+      <c r="N8" s="228"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="76"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="151"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
       <c r="F9" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="151"/>
-      <c r="H9" s="151"/>
-      <c r="I9" s="151"/>
+      <c r="G9" s="229"/>
+      <c r="H9" s="229"/>
+      <c r="I9" s="229"/>
       <c r="J9" s="76" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="76"/>
-      <c r="L9" s="151"/>
-      <c r="M9" s="151"/>
-      <c r="N9" s="152"/>
+      <c r="L9" s="229"/>
+      <c r="M9" s="229"/>
+      <c r="N9" s="230"/>
     </row>
     <row r="10" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="76"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="153"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
-      <c r="I10" s="153"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="227"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="227"/>
       <c r="J10" s="76" t="s">
         <v>7</v>
       </c>
       <c r="K10" s="76"/>
-      <c r="L10" s="151"/>
-      <c r="M10" s="151"/>
-      <c r="N10" s="152"/>
+      <c r="L10" s="229"/>
+      <c r="M10" s="229"/>
+      <c r="N10" s="230"/>
     </row>
     <row r="11" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="26"/>
@@ -7897,44 +7868,44 @@
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="231" t="s">
+      <c r="B13" s="234" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="231" t="s">
+      <c r="C13" s="234" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="231" t="s">
+      <c r="D13" s="234" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="231"/>
-      <c r="F13" s="231" t="s">
+      <c r="E13" s="234"/>
+      <c r="F13" s="234" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="231" t="s">
+      <c r="G13" s="234" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="231" t="s">
+      <c r="H13" s="234" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="231" t="s">
+      <c r="I13" s="234" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="231"/>
-      <c r="K13" s="231"/>
-      <c r="L13" s="231"/>
-      <c r="M13" s="231"/>
-      <c r="N13" s="231" t="s">
+      <c r="J13" s="234"/>
+      <c r="K13" s="234"/>
+      <c r="L13" s="234"/>
+      <c r="M13" s="234"/>
+      <c r="N13" s="234" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="231"/>
-      <c r="C14" s="231"/>
-      <c r="D14" s="231"/>
-      <c r="E14" s="231"/>
-      <c r="F14" s="231"/>
-      <c r="G14" s="231"/>
-      <c r="H14" s="231"/>
+      <c r="B14" s="234"/>
+      <c r="C14" s="234"/>
+      <c r="D14" s="234"/>
+      <c r="E14" s="234"/>
+      <c r="F14" s="234"/>
+      <c r="G14" s="234"/>
+      <c r="H14" s="234"/>
       <c r="I14" s="30" t="s">
         <v>91</v>
       </c>
@@ -7950,13 +7921,13 @@
       <c r="M14" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="N14" s="231"/>
+      <c r="N14" s="234"/>
     </row>
     <row r="15" spans="2:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
-      <c r="D15" s="232"/>
-      <c r="E15" s="232"/>
+      <c r="D15" s="235"/>
+      <c r="E15" s="235"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -7966,8 +7937,8 @@
         <v>1</v>
       </c>
       <c r="C16" s="30"/>
-      <c r="D16" s="229"/>
-      <c r="E16" s="229"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="232"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -7983,8 +7954,8 @@
         <v>2</v>
       </c>
       <c r="C17" s="30"/>
-      <c r="D17" s="229"/>
-      <c r="E17" s="229"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="232"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
@@ -8000,8 +7971,8 @@
         <v>3</v>
       </c>
       <c r="C18" s="30"/>
-      <c r="D18" s="229"/>
-      <c r="E18" s="229"/>
+      <c r="D18" s="232"/>
+      <c r="E18" s="232"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
@@ -8017,8 +7988,8 @@
         <v>4</v>
       </c>
       <c r="C19" s="30"/>
-      <c r="D19" s="229"/>
-      <c r="E19" s="229"/>
+      <c r="D19" s="232"/>
+      <c r="E19" s="232"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>
@@ -8034,8 +8005,8 @@
         <v>5</v>
       </c>
       <c r="C20" s="30"/>
-      <c r="D20" s="229"/>
-      <c r="E20" s="229"/>
+      <c r="D20" s="232"/>
+      <c r="E20" s="232"/>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
       <c r="H20" s="30"/>
@@ -8051,8 +8022,8 @@
         <v>6</v>
       </c>
       <c r="C21" s="30"/>
-      <c r="D21" s="229"/>
-      <c r="E21" s="229"/>
+      <c r="D21" s="232"/>
+      <c r="E21" s="232"/>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -8068,8 +8039,8 @@
         <v>7</v>
       </c>
       <c r="C22" s="30"/>
-      <c r="D22" s="229"/>
-      <c r="E22" s="229"/>
+      <c r="D22" s="232"/>
+      <c r="E22" s="232"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -8085,8 +8056,8 @@
         <v>8</v>
       </c>
       <c r="C23" s="30"/>
-      <c r="D23" s="229"/>
-      <c r="E23" s="229"/>
+      <c r="D23" s="232"/>
+      <c r="E23" s="232"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
@@ -8102,8 +8073,8 @@
         <v>9</v>
       </c>
       <c r="C24" s="30"/>
-      <c r="D24" s="229"/>
-      <c r="E24" s="229"/>
+      <c r="D24" s="232"/>
+      <c r="E24" s="232"/>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30"/>
@@ -8119,8 +8090,8 @@
         <v>10</v>
       </c>
       <c r="C25" s="30"/>
-      <c r="D25" s="229"/>
-      <c r="E25" s="229"/>
+      <c r="D25" s="232"/>
+      <c r="E25" s="232"/>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
@@ -8133,27 +8104,27 @@
     </row>
     <row r="26" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H27" s="233"/>
-      <c r="I27" s="233"/>
-      <c r="J27" s="233"/>
-      <c r="K27" s="233"/>
-      <c r="L27" s="233"/>
+      <c r="H27" s="231"/>
+      <c r="I27" s="231"/>
+      <c r="J27" s="231"/>
+      <c r="K27" s="231"/>
+      <c r="L27" s="231"/>
     </row>
     <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H30" s="233"/>
-      <c r="I30" s="233"/>
-      <c r="J30" s="233"/>
-      <c r="K30" s="233"/>
-      <c r="L30" s="233"/>
+      <c r="H30" s="231"/>
+      <c r="I30" s="231"/>
+      <c r="J30" s="231"/>
+      <c r="K30" s="231"/>
+      <c r="L30" s="231"/>
     </row>
     <row r="31" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H31" s="233"/>
-      <c r="I31" s="233"/>
-      <c r="J31" s="233"/>
-      <c r="K31" s="233"/>
-      <c r="L31" s="233"/>
+      <c r="H31" s="231"/>
+      <c r="I31" s="231"/>
+      <c r="J31" s="231"/>
+      <c r="K31" s="231"/>
+      <c r="L31" s="231"/>
     </row>
     <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32294,14 +32265,12 @@
     <row r="24123" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="D10:I10"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B4:N4"/>
     <mergeCell ref="B13:B14"/>
@@ -32318,12 +32287,14 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H27:L27"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>